<commit_message>
Ajout de la description des argument html
</commit_message>
<xml_diff>
--- a/Data/HtmlCss_list,.xlsx
+++ b/Data/HtmlCss_list,.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="655">
   <si>
     <t>Balise html</t>
   </si>
@@ -1807,12 +1807,973 @@
   <si>
     <t>&lt;button&gt;, &lt;option&gt;, &lt;input&gt;, &lt;li&gt;, &lt;meter&gt;, &lt;progress&gt;, &lt;param&gt;</t>
   </si>
+  <si>
+    <t>La liste des types acceptés par le serveur. Généralement, il s'agit de types de fichier.</t>
+  </si>
+  <si>
+    <t>La liste des jeux de caractères pris en charge.</t>
+  </si>
+  <si>
+    <t>Cet attribut permet de définir un raccourci clavier pour activer un élément ou lui
+ passer le focus.</t>
+  </si>
+  <si>
+    <t>L'URI d'un programme qui traite les informations envoyées par le formulaire.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit l'alignement horizontal de l'élément.</t>
+  </si>
+  <si>
+    <r>
+      <t>Cet attribut définit les règles des fonctionnalités pour cette </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Un texte alternatif à afficher lorsque l'élément ne peut pas être affiché</t>
+  </si>
+  <si>
+    <t>Cet attribut indique que le script devrait être exécuté de façon asynchrone</t>
+  </si>
+  <si>
+    <t>Cet attribut contrôle la façon dont un champ texte est saisi en majuscules 
+de façon automatique.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique que ces contrôles ou que ce formulaire peuvent être remplis automatiquement par le navigateur.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique que l'élément doit recevoir le focus automatiquement
+une fois que la page est chargée.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique que l'élément audio ou vidéo doit être lancé dès que possible.</t>
+  </si>
+  <si>
+    <t>Définit l'URL vers un fichier qui est une image.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique la couleur d'arrière-plan pour l'élément</t>
+  </si>
+  <si>
+    <t>Cet attribut indique la largeur de la bordure.</t>
+  </si>
+  <si>
+    <t>Cet attribut contient la valeur de l'intervalle de temps d'ores et déjà mis en mémoire
+ tampon pour le média de l'élément</t>
+  </si>
+  <si>
+    <t>Une chaîne de challenge qui est envoyée avec la clef publique.</t>
+  </si>
+  <si>
+    <t>Cet attribut déclare l'encodage de caractères utilisé pour la page ou le script</t>
+  </si>
+  <si>
+    <t>Cet attribut indique si l'élément doit être vérifié au chargement de la page.</t>
+  </si>
+  <si>
+    <t>Cet attribut est une URI qui pointe vers la source de la citation ou de la modification</t>
+  </si>
+  <si>
+    <t>Cet attribut permet de définir la ou les classes auxquelles appartient un élément afin de le manipuler en script ou de le mettre en forme avec CSS.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit l'URL du fichier de classe qui doit être utilisé pour le chargement 
+et l'exécution de l'applet.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cet attribut fournit une URL absolue ou relative du dossier contenant les fichiers 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> de l'applet.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cet attribut définit la couleur du texte grâce à un nom de couleur ou grâce
+ à un code hexadécimal dans le format #RRGGBB.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit le nombre de colonnes pour le texte contenu dans un textarea</t>
+  </si>
+  <si>
+    <t>Cet attribut définit le nombre de colonnes sur lequel une cellule doit s'étendre</t>
+  </si>
+  <si>
+    <r>
+      <t>Une valeur associée avec </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>http-equiv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ou </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> selon le contexte.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cet attribut indique si le contenu de l'élément peut être édité.</t>
+  </si>
+  <si>
+    <t>Cet attribut fait référence à l'identifiant d'un élément &lt;menu&gt; qui sera utilisé comme
+ menu contextuel pour l'élément.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique si le navigateur doit afficher les contrôles de lecture du média
+ pour l'utilisateur.</t>
+  </si>
+  <si>
+    <t>Un ensemble de valeurs qui définit les coordonnées de la zone d'intérêt</t>
+  </si>
+  <si>
+    <t>Cet attribut gère les requêtes de différentes origines.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit la politique de sécurité de contenu que le document intégré
+ doit respecter.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit l'URL de la ressource.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grâce aux attributs de donnée, on peut associer des attributs personnalisés afin de transporter des informations spécifiques</t>
+  </si>
+  <si>
+    <t>Cet attribut indique la date et l'heure associées à l'élément.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique la méthode préférée pour décoder l'image.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique que la piste devrait être activée sauf si les préférences
+ de l'utilisateur indique un autre choi</t>
+  </si>
+  <si>
+    <t>Cet attribut indique que le script doit être exécuté une fois que la page 
+a été analysée.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit la direction du texte (gauche à droite ou droite à gauche).</t>
+  </si>
+  <si>
+    <t>Cet attribut indique si l'utilisateur peut interagir avec l'élément.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique si l'hyperlien est utilisé afin de télécharger une ressource.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique si l'élément peut être déplacé/glissé</t>
+  </si>
+  <si>
+    <t>Cet attribut indique si l'élément peut recevoir du contenu suite à un glisser/déposer.</t>
+  </si>
+  <si>
+    <r>
+      <t>Cet attribut définit le type de contenu des données de formulaire envoyées 
+lorsque la méthode utilisée est </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>POST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Cet attribut indique le libellé ou l'icône à afficher sur la touche entrée des clavier virtuels. Cet attribut peut être utilisé sur les contrôles de formulaires ou sur les éléments qui sont éditables (par exemple avec l'attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>contenteditable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">).
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Cet attribut décrit l'élément auquel se rapporte l'élément courant.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique le formulaire auquel l'élément se rapporte.</t>
+  </si>
+  <si>
+    <r>
+      <t>Cet attribut est l'URI du programme qui traite les données pour ces champs 
+du formulaire. Il prend le pas sur l'attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>action</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> défini pour &lt;form&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Si le bouton ou le champ sert à l'envoi (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type="submit"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>), cet attribut indique 
+l'encodage utilisé pour l'envoi des données. Si cet attribut est indiqué, il surcharge
+ l'attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>enctype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> du formulaire auquel est rattaché le bouton/champ.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Si le bouton ou le champ sert à l'envoi (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type="submit"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>), cet attribut indique
+ la méthode HTTP pour envoyer les données (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>POST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, etc.). Si cet attribut
+ est indiqué, il surcharge l'attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>method</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> du formulaire auquel est rattaché
+ le bouton/champ.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Si le bouton ou le champ sert à l'envoi (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type="submit"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>), cet attribut booléen
+ indique que le formulaire ne doit pas être validé à l'envoi. Si cet attribut est 
+indiqué, il surcharge l'attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>novalidate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> du formulaire auquel est rattaché
+ le bouton/champ.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Si le bouton ou le champ sert à l'envoi (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type="submit"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>), cet attribut indique 
+le contexte de navigation (onglet, fenêtre ou </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) dans lequel afficher
+ la réponse après l'envoi du formulaire. Si cet attribut est indiqué, 
+il surcharge l'attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> du formulaire auquel est rattaché le bouton/champ.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Les identifiants des éléments </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;th&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> qui s'appliquent à cet élément.</t>
+    </r>
+  </si>
+  <si>
+    <t>Pour ces éléments, cet attribut définit la hauteur occupée par l'élément. 
+Pour les autres éléments, on utilisera height proprety.</t>
+  </si>
+  <si>
+    <t>Cet attribut empêche le rendu d'un élément sur une page tout en conservant 
+les éléments fils actifs.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique la borne inférieure de l'intervalle haut.</t>
+  </si>
+  <si>
+    <t>L'URL de la ressource liée.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique la langue utilisé pour la ressource liée.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique une image qui représente la commande.</t>
+  </si>
+  <si>
+    <t>Cet attribut permet d'identifier un élément d'un document de façon unique.
+ Il est généralement utilisé pour manipuler l'élément avec des scripts ou pour
+ le mettre en forme avec CSS.</t>
+  </si>
+  <si>
+    <r>
+      <t>Cet attribut indique la priorité relative pour la récupération (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>fetch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) des ressources.</t>
+    </r>
+  </si>
+  <si>
+    <t>Une fonctionnalité relative à la sécurité qui permet aux navigateurs de vérifier les
+ fichiers qu'ils récupèrent.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique au navigateur qu'il faut ignorer la taille intrinsèque 
+de l'image et qu'il faut utiliser la taille indiquée avec les attributs.</t>
+  </si>
+  <si>
+    <r>
+      <t>Cet attribut fournit une indication sur le type de donnée qui pourrait être saisi 
+par l'utilisateur lors de l'édition du formulaire ou de l'élément. Cet attribut peut être
+ utilisé sur les contrôles de formulaires ou sur les éléments qui sont éditables 
+(par exemple avec l'attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>contenteditable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <t>Cet attribut indique que l'image contribue à une mosaïque d'images interactive
+ côté serveur.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit le type de clé qui est généré.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit le type de piste textuelle.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit un titre, lisible par un utilisateur, pour l'élément.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit la langue utilisée dans l'élément.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit le langage de script utilisé dans l'élément.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique que l'élément doit être chargé à la demande.</t>
+  </si>
+  <si>
+    <t>Cet attribut constitue une liste d'options prédéfinie qui est suggérée à l'utilisateur.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique si le média courant doit recommencer au début une fois que 
+sa lecture est terminée.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique la borne supérieure de l'intervalle bas.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit l'URL du manifeste du document pour la gestion du cache.On utilise maintenant &lt;link rel="manifest"&gt;</t>
+  </si>
+  <si>
+    <t>Cet attribut indique la valeur maximale autorisée.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit le nombre maximal de caractères autorisé dans l'élément.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit le nombre minimal de caractères qui doivent être saisis dans
+ l'élément.</t>
+  </si>
+  <si>
+    <t>Cet attribut est indication à propos du type de média pour la ressource liée.</t>
+  </si>
+  <si>
+    <t>Cet attriput défini par la méthode HTTPà utiliser pour l'envoi des données 
+du formulaire (GET par défaut ou POST)</t>
+  </si>
+  <si>
+    <t>Cet attribut indique la valeur minimale autorisée.</t>
+  </si>
+  <si>
+    <r>
+      <t>Cet attribut indique si plusieurs valeurs peuvent être saisies pour des entrées 
+de type </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ou </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cet attribut indique si le son de la vidéo doit être coupé lorsque la page est 
+chargée initialement.</t>
+  </si>
+  <si>
+    <t>Le nom de l'élément qui peut être utilisé par le serveur pour identifier le champ 
+d'un formulaire.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique que les données du formulaire ne doivent pas être validées
+ lors de l'envoi</t>
+  </si>
+  <si>
+    <t>Cet attribut indique si les détails seront affichés lors du chargement de la page</t>
+  </si>
+  <si>
+    <t>Cet attribut indique la valeur numérique optimale.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit une expression rationnelle contre laquelle valider la valeur 
+de l'élément.</t>
+  </si>
+  <si>
+    <t>Cet attribut fournit une indication à l'utilisateur sur ce qu'il peut saisir dans le champ.</t>
+  </si>
+  <si>
+    <t>Cet attribut est une URL qui indique l'image à afficher tant que l'utilisateur n'a pas lancé la vidéo ou déplacé le curseur.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique si toute ou partie, voire aucune partie de la ressource doit être 
+téléchargée en avance.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique si l'élément peut être édité.</t>
+  </si>
+  <si>
+    <r>
+      <t>Définit le référent (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>referrer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) envoyé lors de la récupération de la ressource.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cet attribut définit la relation entre l'objet cible et l'objet du lien.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique si l'élément doit obligatoirement être renseigné dans le formulaire.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique si la liste doit être affichée dans un ordre décroissant plutôt 
+que dans un ordre croissant.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit le nombre de lignes pour la zone de texte.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit le nombre de lignes sur lesquelles une cellule doit s'étendre.</t>
+  </si>
+  <si>
+    <r>
+      <t>Empêche un élément chargé dans une </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>iframe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> d'utiliser certaines fonctionnalités (envoyer des formulaires ou ouvrir de nouvelles fenêtres par exemples).</t>
+    </r>
+  </si>
+  <si>
+    <t>Définit les cellules sur lesquelles porte la cellule d'en-tête.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit la valeur qui sera sélectionnée au chargement de la page.</t>
+  </si>
+  <si>
+    <r>
+      <t>Cet attribut définit la largeur de l'élément en pixels, si l'attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> de l'élément 
+vaut </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>text</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ou </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>password</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, cela correspond au nombre de caractères du champ.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Cet attribut affecte un créneau pour un élément dans le </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>shadow DOM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cet attribut indique si la vérification orthographique est activée pour l'élément courant.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique l'URL du contenu embarqué.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit le première nombre de la liste si celui-ci est différent de 1.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit des styles CSS qui auront la priorité sur ceux définis 
+précédemment. Il ne devrait être utilisé qu'à des fins de tests car il est conseillé 
+d'utiliser un/des fichier(s) à part pour gérer la mise en forme.</t>
+  </si>
+  <si>
+    <t>Cet attribut permet de modifier l'ordre dans la navigation à la tabulation.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit un texte expliquant le contenu de l'élément et qui est généralement
+ affiché sous la forme d'une bulle d'information au survol de l'élément.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique si le contenu textuel de l'élément doit être traduit ou non.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit le type de l'élément.</t>
+  </si>
+  <si>
+    <t>Cet attribut définit la valeur par défaut qui sera affichée dans l'élément au 
+chargement de la page.</t>
+  </si>
+  <si>
+    <t>Pour ces éléments, cet attribut définit la largeur occupée sur l'écran.</t>
+  </si>
+  <si>
+    <t>Cet attribut indique l'utilisation du retour automatique à la ligne pour le texte de 
+l'élément.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1820,16 +2781,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1837,14 +2823,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3673,15 +4707,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="103.5546875" customWidth="1"/>
-    <col min="3" max="3" width="62.44140625" customWidth="1"/>
+    <col min="3" max="3" width="69.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -3705,6 +4739,9 @@
       <c r="B2" t="s">
         <v>493</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>540</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -3713,13 +4750,19 @@
       <c r="B3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>369</v>
       </c>
       <c r="B4" t="s">
         <v>494</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3729,6 +4772,9 @@
       <c r="B5" t="s">
         <v>37</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -3737,6 +4783,9 @@
       <c r="B6" t="s">
         <v>495</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -3745,45 +4794,63 @@
       <c r="B7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C7" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>373</v>
       </c>
       <c r="B8" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>374</v>
       </c>
       <c r="B9" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="4" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>375</v>
       </c>
       <c r="B10" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C10" s="6" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>376</v>
       </c>
       <c r="B11" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="4" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>377</v>
       </c>
       <c r="B12" t="s">
         <v>498</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -3793,6 +4860,9 @@
       <c r="B13" t="s">
         <v>499</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>551</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -3801,6 +4871,9 @@
       <c r="B14" t="s">
         <v>500</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -3809,6 +4882,9 @@
       <c r="B15" t="s">
         <v>501</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -3817,208 +4893,286 @@
       <c r="B16" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>380</v>
       </c>
       <c r="B17" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="8" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>381</v>
       </c>
       <c r="B18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="4" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>382</v>
       </c>
       <c r="B19" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>383</v>
       </c>
       <c r="B20" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="2" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>384</v>
       </c>
       <c r="B21" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" s="2" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>385</v>
       </c>
       <c r="B22" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" s="4" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>386</v>
       </c>
       <c r="B23" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" s="8" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>387</v>
       </c>
       <c r="B24" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" s="8" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>274</v>
       </c>
       <c r="B25" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" s="8" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>388</v>
       </c>
       <c r="B26" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>389</v>
       </c>
       <c r="B27" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" s="4" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>390</v>
       </c>
       <c r="B28" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>391</v>
       </c>
       <c r="B29" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>392</v>
       </c>
       <c r="B30" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" s="8" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>393</v>
       </c>
       <c r="B31" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" s="8" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>394</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" s="2" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>395</v>
       </c>
       <c r="B33" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>396</v>
       </c>
       <c r="B34" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" s="8" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>397</v>
       </c>
       <c r="B35" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>398</v>
       </c>
       <c r="B36" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" s="4" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>399</v>
       </c>
       <c r="B37" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" s="2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>400</v>
       </c>
       <c r="B38" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>401</v>
       </c>
       <c r="B39" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39" s="8" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>402</v>
       </c>
       <c r="B40" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40" s="8" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>403</v>
       </c>
       <c r="B41" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>404</v>
       </c>
@@ -4026,159 +5180,216 @@
         <v>512</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>405</v>
       </c>
       <c r="B43" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43" s="2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>406</v>
       </c>
       <c r="B44" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44" s="4" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>407</v>
       </c>
       <c r="B45" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>408</v>
       </c>
       <c r="B46" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>409</v>
       </c>
       <c r="B47" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47" s="8" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>410</v>
       </c>
       <c r="B48" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48" s="8" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>411</v>
       </c>
       <c r="B49" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49" s="4" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>412</v>
       </c>
       <c r="B50" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50" s="2" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>413</v>
       </c>
       <c r="B51" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51" s="8" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>414</v>
       </c>
       <c r="B52" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52" s="8" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>415</v>
       </c>
       <c r="B53" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53" s="8" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>416</v>
       </c>
       <c r="B54" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54" s="8" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>417</v>
       </c>
       <c r="B55" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55" s="8" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>418</v>
       </c>
       <c r="B56" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>282</v>
       </c>
       <c r="B57" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57" s="8" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>419</v>
       </c>
       <c r="B58" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58" s="8" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>420</v>
       </c>
       <c r="B59" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59" s="2" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>421</v>
       </c>
       <c r="B60" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60" s="4" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>422</v>
       </c>
       <c r="B61" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61" s="2" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>423</v>
       </c>
@@ -4186,63 +5397,84 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>424</v>
       </c>
       <c r="B63" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63" s="2" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>425</v>
       </c>
       <c r="B64" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64" s="8" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>426</v>
       </c>
       <c r="B65" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65" s="2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>427</v>
       </c>
       <c r="B66" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66" s="8" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>428</v>
       </c>
       <c r="B67" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67" s="8" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>429</v>
       </c>
       <c r="B68" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68" s="8" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>430</v>
       </c>
       <c r="B69" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69" s="8" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>431</v>
       </c>
@@ -4250,191 +5482,260 @@
         <v>494</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>432</v>
       </c>
       <c r="B71" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71" s="2" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>433</v>
       </c>
       <c r="B72" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72" s="4" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>434</v>
       </c>
       <c r="B73" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C73" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>435</v>
       </c>
       <c r="B74" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>436</v>
       </c>
       <c r="B75" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C75" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>437</v>
       </c>
       <c r="B76" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76" s="2" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>438</v>
       </c>
       <c r="B77" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C77" s="2" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>439</v>
       </c>
       <c r="B78" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C78" s="8" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>440</v>
       </c>
       <c r="B79" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C79" s="2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>441</v>
       </c>
       <c r="B80" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C80" s="9" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>442</v>
       </c>
       <c r="B81" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C81" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>443</v>
       </c>
       <c r="B82" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C82" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>444</v>
       </c>
       <c r="B83" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C83" s="8" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>445</v>
       </c>
       <c r="B84" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C84" s="2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>446</v>
       </c>
       <c r="B85" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C85" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>447</v>
       </c>
       <c r="B86" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C86" s="2" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>448</v>
       </c>
       <c r="B87" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C87" s="8" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>449</v>
       </c>
       <c r="B88" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C88" s="8" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>450</v>
       </c>
       <c r="B89" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C89" s="8" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>451</v>
       </c>
       <c r="B90" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C90" s="8" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>452</v>
       </c>
       <c r="B91" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C91" s="4" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>453</v>
       </c>
       <c r="B92" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C92" s="4" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>454</v>
       </c>
       <c r="B93" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C93" s="8" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>455</v>
       </c>
@@ -4442,31 +5743,40 @@
         <v>514</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>456</v>
       </c>
       <c r="B95" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C95" s="2" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>457</v>
       </c>
       <c r="B96" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C96" s="4" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>458</v>
       </c>
       <c r="B97" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C97" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>459</v>
       </c>
@@ -4474,79 +5784,106 @@
         <v>22</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>460</v>
       </c>
       <c r="B99" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C99" s="2" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>461</v>
       </c>
       <c r="B100" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C100" s="2" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>462</v>
       </c>
       <c r="B101" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C101" s="4" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>463</v>
       </c>
       <c r="B102" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C102" s="2" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>464</v>
       </c>
       <c r="B103" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C103" s="8" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>465</v>
       </c>
       <c r="B104" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C104" s="2" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>466</v>
       </c>
       <c r="B105" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C105" s="2" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>467</v>
       </c>
       <c r="B106" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C106" s="4" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>468</v>
       </c>
       <c r="B107" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C107" s="2" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>469</v>
       </c>
@@ -4554,15 +5891,18 @@
         <v>86</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>470</v>
       </c>
       <c r="B109" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C109" s="4" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>471</v>
       </c>
@@ -4570,15 +5910,18 @@
         <v>514</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>472</v>
       </c>
       <c r="B111" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C111" s="8" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>473</v>
       </c>
@@ -4586,15 +5929,18 @@
         <v>533</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>474</v>
       </c>
       <c r="B113" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C113" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>475</v>
       </c>
@@ -4602,23 +5948,29 @@
         <v>534</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>476</v>
       </c>
       <c r="B115" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C115" s="2" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>477</v>
       </c>
       <c r="B116" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C116" s="2" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>478</v>
       </c>
@@ -4626,7 +5978,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>479</v>
       </c>
@@ -4634,7 +5986,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>480</v>
       </c>
@@ -4642,15 +5994,18 @@
         <v>51</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>481</v>
       </c>
       <c r="B120" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C120" s="4" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>482</v>
       </c>
@@ -4658,15 +6013,18 @@
         <v>52</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>483</v>
       </c>
       <c r="B122" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C122" s="8" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>484</v>
       </c>
@@ -4674,15 +6032,18 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>485</v>
       </c>
       <c r="B124" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C124" s="2" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>486</v>
       </c>
@@ -4690,60 +6051,79 @@
         <v>536</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>487</v>
       </c>
       <c r="B126" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C126" s="8" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>488</v>
       </c>
       <c r="B127" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C127" s="4" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>489</v>
       </c>
       <c r="B128" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C128" s="4" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>490</v>
       </c>
       <c r="B129" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C129" s="5"/>
+    </row>
+    <row r="130" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>491</v>
       </c>
       <c r="B130" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C130" s="8" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>281</v>
       </c>
       <c r="B131" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C131" s="2" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>492</v>
       </c>
       <c r="B132" t="s">
         <v>508</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>654</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Premier ébauche des mots dans le dossier data
</commit_message>
<xml_diff>
--- a/Data/HtmlCss_list,.xlsx
+++ b/Data/HtmlCss_list,.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HTML_list-tag" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="739">
   <si>
     <t>Balise html</t>
   </si>
@@ -2767,6 +2767,264 @@
   <si>
     <t>Cet attribut indique l'utilisation du retour automatique à la ligne pour le texte de 
 l'élément.</t>
+  </si>
+  <si>
+    <t>lien, redirection</t>
+  </si>
+  <si>
+    <t>abréviation</t>
+  </si>
+  <si>
+    <t>écris (footer), marquer</t>
+  </si>
+  <si>
+    <t>zone, espace</t>
+  </si>
+  <si>
+    <t>ajoute</t>
+  </si>
+  <si>
+    <t>fichier audio,
+ enregistrement</t>
+  </si>
+  <si>
+    <t>en, gras
+paragraphe</t>
+  </si>
+  <si>
+    <t>longue citation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a la ligne </t>
+  </si>
+  <si>
+    <t>bouton</t>
+  </si>
+  <si>
+    <t>graphique, shéma</t>
+  </si>
+  <si>
+    <t>Titre au tableau</t>
+  </si>
+  <si>
+    <t>Titre</t>
+  </si>
+  <si>
+    <t>colonne</t>
+  </si>
+  <si>
+    <t>groupe de colonne</t>
+  </si>
+  <si>
+    <t>liste déroulante</t>
+  </si>
+  <si>
+    <t>définition</t>
+  </si>
+  <si>
+    <t>Dans un cadre</t>
+  </si>
+  <si>
+    <t>mettre en emphase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plug-in </t>
+  </si>
+  <si>
+    <t>regroupe</t>
+  </si>
+  <si>
+    <t>description, légende</t>
+  </si>
+  <si>
+    <t>formulaire</t>
+  </si>
+  <si>
+    <t>en grand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sous fenetre,
+implemente
+</t>
+  </si>
+  <si>
+    <t>image, photo</t>
+  </si>
+  <si>
+    <t>lien</t>
+  </si>
+  <si>
+    <t>carte</t>
+  </si>
+  <si>
+    <t>surligne</t>
+  </si>
+  <si>
+    <t>objet</t>
+  </si>
+  <si>
+    <t>liste ordonée</t>
+  </si>
+  <si>
+    <t>groupe + liste 
+déroulente</t>
+  </si>
+  <si>
+    <t>item +liste
+déroulente</t>
+  </si>
+  <si>
+    <t>sortie, égal</t>
+  </si>
+  <si>
+    <t>écris, paragraphe</t>
+  </si>
+  <si>
+    <t>barre de prgression</t>
+  </si>
+  <si>
+    <t>citation</t>
+  </si>
+  <si>
+    <t>code, script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">réduis, </t>
+  </si>
+  <si>
+    <t>qui se diférencie</t>
+  </si>
+  <si>
+    <t>en gras</t>
+  </si>
+  <si>
+    <t>tableau</t>
+  </si>
+  <si>
+    <t>cellule, case</t>
+  </si>
+  <si>
+    <t>titre</t>
+  </si>
+  <si>
+    <t>temps, entre</t>
+  </si>
+  <si>
+    <t>liste a puce</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>retour a la ligne</t>
+  </si>
+  <si>
+    <t>police, écriture</t>
+  </si>
+  <si>
+    <t>taille, text,grand,petit</t>
+  </si>
+  <si>
+    <t>gras</t>
+  </si>
+  <si>
+    <t>italique</t>
+  </si>
+  <si>
+    <t>souligne, barre, clignote</t>
+  </si>
+  <si>
+    <t>petite lettre</t>
+  </si>
+  <si>
+    <t>capitale</t>
+  </si>
+  <si>
+    <t>aligne + direction</t>
+  </si>
+  <si>
+    <t>alignement + haut/bas</t>
+  </si>
+  <si>
+    <t>hauteur + ligne</t>
+  </si>
+  <si>
+    <t>alinéa, espace</t>
+  </si>
+  <si>
+    <t>césurre</t>
+  </si>
+  <si>
+    <t>couleur +text</t>
+  </si>
+  <si>
+    <t>couleur + arrière + fond</t>
+  </si>
+  <si>
+    <t>image + arrière/fond</t>
+  </si>
+  <si>
+    <t>répete fond</t>
+  </si>
+  <si>
+    <t>fond + direction</t>
+  </si>
+  <si>
+    <t>largeur</t>
+  </si>
+  <si>
+    <t>hauteur</t>
+  </si>
+  <si>
+    <t>largeur maximimu abv</t>
+  </si>
+  <si>
+    <t>largeur minimum abv</t>
+  </si>
+  <si>
+    <t>hauter minimum abv</t>
+  </si>
+  <si>
+    <t>jeuteur maximum abv</t>
+  </si>
+  <si>
+    <t>marge +direction</t>
+  </si>
+  <si>
+    <t>idem</t>
+  </si>
+  <si>
+    <t>marge interieur +direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> épaisseur bordure</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> couleur bordure</t>
+  </si>
+  <si>
+    <t>bordure direction</t>
+  </si>
+  <si>
+    <t>masqué, caché</t>
+  </si>
+  <si>
+    <t>flotant direction</t>
+  </si>
+  <si>
+    <t>position +direction</t>
+  </si>
+  <si>
+    <t>ordre affichage</t>
+  </si>
+  <si>
+    <t>liste ( )</t>
+  </si>
+  <si>
+    <t>barre de défilement</t>
   </si>
 </sst>
 </file>
@@ -3162,14 +3420,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.21875" customWidth="1"/>
     <col min="2" max="2" width="165.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -3198,6 +3457,9 @@
       <c r="B3" t="s">
         <v>107</v>
       </c>
+      <c r="C3" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -3206,6 +3468,9 @@
       <c r="B4" t="s">
         <v>108</v>
       </c>
+      <c r="C4" t="s">
+        <v>656</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -3214,6 +3479,9 @@
       <c r="B5" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="C5" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -3222,6 +3490,9 @@
       <c r="B6" t="s">
         <v>110</v>
       </c>
+      <c r="C6" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -3230,6 +3501,9 @@
       <c r="B7" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="C7" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -3239,12 +3513,15 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>113</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>660</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -3254,6 +3531,9 @@
       <c r="B10" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>661</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -3270,6 +3550,9 @@
       <c r="B12" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="C12" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -3286,6 +3569,9 @@
       <c r="B14" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="C14" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -3294,6 +3580,9 @@
       <c r="B15" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="C15" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -3302,24 +3591,33 @@
       <c r="B16" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -3327,39 +3625,51 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3367,7 +3677,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -3375,7 +3685,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -3383,7 +3693,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -3391,63 +3701,84 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -3455,7 +3786,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -3463,23 +3794,29 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -3487,7 +3824,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -3495,7 +3832,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -3503,7 +3840,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -3511,7 +3848,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -3519,7 +3856,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -3527,7 +3864,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -3535,7 +3872,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -3543,7 +3880,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -3551,7 +3888,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -3559,7 +3896,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -3567,23 +3904,29 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -3591,7 +3934,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -3599,7 +3942,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -3607,7 +3950,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -3615,7 +3958,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -3623,7 +3966,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -3631,7 +3974,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -3639,31 +3982,40 @@
         <v>157</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -3671,7 +4023,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -3679,7 +4031,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -3687,7 +4039,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -3695,7 +4047,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -3703,55 +4055,73 @@
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69" s="1" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C70" s="1" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -3759,7 +4129,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -3767,23 +4137,29 @@
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -3791,7 +4167,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -3799,15 +4175,18 @@
         <v>177</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -3815,23 +4194,29 @@
         <v>179</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>81</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>82</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -3839,23 +4224,29 @@
         <v>181</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>84</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C84" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>85</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C85" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -3863,7 +4254,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -3871,7 +4262,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -3879,7 +4270,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -3887,15 +4278,18 @@
         <v>187</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>90</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C90" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -3903,15 +4297,18 @@
         <v>189</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>92</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C92" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -3919,7 +4316,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>94</v>
       </c>
@@ -3927,7 +4324,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -3935,7 +4332,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>96</v>
       </c>
@@ -3943,15 +4340,18 @@
         <v>194</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>97</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C97" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>98</v>
       </c>
@@ -3959,7 +4359,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -3967,44 +4367,59 @@
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>100</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C100" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>101</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C101" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>102</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C102" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>103</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C103" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>104</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>202</v>
+      </c>
+      <c r="C104" t="s">
+        <v>703</v>
       </c>
     </row>
   </sheetData>
@@ -4016,8 +4431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4025,6 +4440,7 @@
     <col min="1" max="1" width="25.88671875" customWidth="1"/>
     <col min="2" max="2" width="21.21875" customWidth="1"/>
     <col min="3" max="3" width="77.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -4051,6 +4467,9 @@
       <c r="C2" s="1" t="s">
         <v>321</v>
       </c>
+      <c r="D2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -4062,6 +4481,9 @@
       <c r="C3" s="1" t="s">
         <v>322</v>
       </c>
+      <c r="D3" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -4073,6 +4495,9 @@
       <c r="C4" s="1" t="s">
         <v>323</v>
       </c>
+      <c r="D4" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -4084,6 +4509,9 @@
       <c r="C5" s="1" t="s">
         <v>324</v>
       </c>
+      <c r="D5" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -4095,6 +4523,9 @@
       <c r="C6" s="1" t="s">
         <v>325</v>
       </c>
+      <c r="D6" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -4106,6 +4537,9 @@
       <c r="C7" s="1" t="s">
         <v>326</v>
       </c>
+      <c r="D7" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -4117,6 +4551,9 @@
       <c r="C8" s="1" t="s">
         <v>327</v>
       </c>
+      <c r="D8" t="s">
+        <v>710</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -4128,6 +4565,9 @@
       <c r="C9" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="D9" t="s">
+        <v>711</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -4139,6 +4579,9 @@
       <c r="C10" s="1" t="s">
         <v>329</v>
       </c>
+      <c r="D10" t="s">
+        <v>712</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -4150,6 +4593,9 @@
       <c r="C11" t="s">
         <v>330</v>
       </c>
+      <c r="D11" t="s">
+        <v>713</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -4161,6 +4607,9 @@
       <c r="C12" s="1" t="s">
         <v>331</v>
       </c>
+      <c r="D12" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -4172,6 +4621,9 @@
       <c r="C13" s="1" t="s">
         <v>332</v>
       </c>
+      <c r="D13" t="s">
+        <v>715</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -4183,6 +4635,9 @@
       <c r="C14" s="1" t="s">
         <v>333</v>
       </c>
+      <c r="D14" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -4194,6 +4649,9 @@
       <c r="C15" t="s">
         <v>334</v>
       </c>
+      <c r="D15" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -4205,8 +4663,11 @@
       <c r="C16" s="1" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>221</v>
       </c>
@@ -4217,7 +4678,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>222</v>
       </c>
@@ -4227,8 +4688,11 @@
       <c r="C18" s="1" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>223</v>
       </c>
@@ -4238,8 +4702,11 @@
       <c r="C19" s="1" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>224</v>
       </c>
@@ -4250,7 +4717,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>225</v>
       </c>
@@ -4260,8 +4727,11 @@
       <c r="C21" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>226</v>
       </c>
@@ -4271,8 +4741,11 @@
       <c r="C22" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>227</v>
       </c>
@@ -4282,8 +4755,11 @@
       <c r="C23" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>228</v>
       </c>
@@ -4293,8 +4769,11 @@
       <c r="C24" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>229</v>
       </c>
@@ -4304,8 +4783,11 @@
       <c r="C25" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>230</v>
       </c>
@@ -4315,8 +4797,11 @@
       <c r="C26" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>231</v>
       </c>
@@ -4326,8 +4811,11 @@
       <c r="C27" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>232</v>
       </c>
@@ -4337,8 +4825,11 @@
       <c r="C28" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>233</v>
       </c>
@@ -4348,8 +4839,11 @@
       <c r="C29" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>234</v>
       </c>
@@ -4359,8 +4853,11 @@
       <c r="C30" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>224</v>
       </c>
@@ -4371,7 +4868,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>235</v>
       </c>
@@ -4381,8 +4878,11 @@
       <c r="C32" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>236</v>
       </c>
@@ -4392,8 +4892,11 @@
       <c r="C33" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>237</v>
       </c>
@@ -4403,8 +4906,11 @@
       <c r="C34" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>238</v>
       </c>
@@ -4414,8 +4920,11 @@
       <c r="C35" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>224</v>
       </c>
@@ -4426,7 +4935,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>239</v>
       </c>
@@ -4436,8 +4945,11 @@
       <c r="C37" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>240</v>
       </c>
@@ -4447,8 +4959,11 @@
       <c r="C38" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>241</v>
       </c>
@@ -4459,7 +4974,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>242</v>
       </c>
@@ -4469,8 +4984,11 @@
       <c r="C40" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>243</v>
       </c>
@@ -4480,8 +4998,11 @@
       <c r="C41" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>244</v>
       </c>
@@ -4491,8 +5012,11 @@
       <c r="C42" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>245</v>
       </c>
@@ -4502,8 +5026,11 @@
       <c r="C43" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -4514,7 +5041,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>246</v>
       </c>
@@ -4525,7 +5052,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>247</v>
       </c>
@@ -4535,8 +5062,11 @@
       <c r="C46" s="1" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>248</v>
       </c>
@@ -4547,7 +5077,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>249</v>
       </c>
@@ -4557,8 +5087,11 @@
       <c r="C48" s="1" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>250</v>
       </c>
@@ -4569,7 +5102,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>251</v>
       </c>
@@ -4580,7 +5113,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>252</v>
       </c>
@@ -4590,8 +5123,11 @@
       <c r="C51" s="1" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>253</v>
       </c>
@@ -4601,8 +5137,11 @@
       <c r="C52" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>254</v>
       </c>
@@ -4612,8 +5151,11 @@
       <c r="C53" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>255</v>
       </c>
@@ -4623,8 +5165,11 @@
       <c r="C54" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>256</v>
       </c>
@@ -4634,8 +5179,11 @@
       <c r="C55" s="1" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="216" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>257</v>
       </c>
@@ -4645,8 +5193,11 @@
       <c r="C56" s="1" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>258</v>
       </c>
@@ -4657,7 +5208,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>259</v>
       </c>
@@ -4668,7 +5219,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>224</v>
       </c>
@@ -4679,7 +5230,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>260</v>
       </c>
@@ -4690,12 +5241,15 @@
         <v>362</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>261</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>363</v>
+      </c>
+      <c r="D61" t="s">
+        <v>738</v>
       </c>
     </row>
   </sheetData>
@@ -4707,7 +5261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+    <sheetView topLeftCell="A111" workbookViewId="0">
       <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>

</xml_diff>